<commit_message>
Save results of downhill function
</commit_message>
<xml_diff>
--- a/Data_alloc_change_on_target_change_comp_NM_large_problem_test.xlsx
+++ b/Data_alloc_change_on_target_change_comp_NM_large_problem_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>DATASET</t>
   </si>
@@ -389,7 +389,7 @@
   <dimension ref="A1:AK60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -612,46 +612,19 @@
       <c r="AI3" s="1"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E4" s="1">
-        <f>D4*0.3</f>
-        <v>1200</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>300</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I4" s="1">
-        <v>450</v>
-      </c>
-      <c r="J4" s="1">
-        <v>800</v>
-      </c>
-      <c r="K4" s="1">
-        <v>200</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -676,46 +649,19 @@
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E5" s="1">
-        <f>D5*0.4</f>
-        <v>1600</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G5" s="1">
-        <v>300</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I5" s="1">
-        <v>450</v>
-      </c>
-      <c r="J5" s="1">
-        <v>800</v>
-      </c>
-      <c r="K5" s="1">
-        <v>200</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -740,46 +686,19 @@
       <c r="AI5" s="1"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E6" s="1">
-        <f>D6*0.5</f>
-        <v>2000</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="1">
-        <v>300</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I6" s="1">
-        <v>450</v>
-      </c>
-      <c r="J6" s="1">
-        <v>800</v>
-      </c>
-      <c r="K6" s="1">
-        <v>200</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -804,46 +723,19 @@
       <c r="AI6" s="1"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E7" s="1">
-        <f>D7*0.6</f>
-        <v>2400</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="1">
-        <v>300</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I7" s="1">
-        <v>450</v>
-      </c>
-      <c r="J7" s="1">
-        <v>800</v>
-      </c>
-      <c r="K7" s="1">
-        <v>200</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -868,46 +760,19 @@
       <c r="AI7" s="1"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E8" s="1">
-        <f>D8*0.7</f>
-        <v>2800</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G8" s="1">
-        <v>300</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I8" s="1">
-        <v>450</v>
-      </c>
-      <c r="J8" s="1">
-        <v>800</v>
-      </c>
-      <c r="K8" s="1">
-        <v>200</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -932,46 +797,19 @@
       <c r="AI8" s="1"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E9" s="1">
-        <f>D9*0.8</f>
-        <v>3200</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G9" s="1">
-        <v>300</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I9" s="1">
-        <v>450</v>
-      </c>
-      <c r="J9" s="1">
-        <v>800</v>
-      </c>
-      <c r="K9" s="1">
-        <v>200</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -996,46 +834,19 @@
       <c r="AI9" s="1"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E10" s="1">
-        <f>D10*0.9</f>
-        <v>3600</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G10" s="1">
-        <v>300</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I10" s="1">
-        <v>450</v>
-      </c>
-      <c r="J10" s="1">
-        <v>800</v>
-      </c>
-      <c r="K10" s="1">
-        <v>200</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1060,46 +871,19 @@
       <c r="AI10" s="1"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E11" s="1">
-        <f>D11*0.95</f>
-        <v>3800</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G11" s="1">
-        <v>300</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I11" s="1">
-        <v>450</v>
-      </c>
-      <c r="J11" s="1">
-        <v>800</v>
-      </c>
-      <c r="K11" s="1">
-        <v>200</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>

</xml_diff>

<commit_message>
Added support for triangular distribution
</commit_message>
<xml_diff>
--- a/Data_alloc_change_on_target_change_comp_NM_large_problem_test.xlsx
+++ b/Data_alloc_change_on_target_change_comp_NM_large_problem_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>DATASET</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>uniform</t>
+  </si>
+  <si>
+    <t>triang</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
   <dimension ref="A1:AK60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -613,19 +616,45 @@
       <c r="AI3" s="1"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2800</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1800</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>

</xml_diff>